<commit_message>
feat: add VBA code sheet and FRM April analysis script
- Add VBA_Code sheet with complete macros for library loading
- Create frm_april_analysis.py for FRM meeting scenarios
- Generate FRM_April_Analysis.xlsx with 3 scenarios x 2 cost variations
- Update BESS_Analyzer.xlsx with 8 sheets including VBA instructions

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bess_analyzer/BESS_Analyzer.xlsx
+++ b/bess_analyzer/BESS_Analyzer.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Sensitivity" sheetId="5" r:id="rId5"/>
     <sheet name="Methodology" sheetId="6" r:id="rId6"/>
     <sheet name="Library_Data" sheetId="7" r:id="rId7"/>
+    <sheet name="VBA_Code" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Analysis_Years">Inputs!$C$13</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="583">
   <si>
     <t>BESS Economic Analysis - Project Inputs</t>
   </si>
@@ -961,6 +962,822 @@
   </si>
   <si>
     <t>Voltage Support [common]</t>
+  </si>
+  <si>
+    <t>VBA Macro Code &amp; Setup Instructions</t>
+  </si>
+  <si>
+    <t>STEP-BY-STEP INSTRUCTIONS TO ENABLE MACROS</t>
+  </si>
+  <si>
+    <t>Step 1:</t>
+  </si>
+  <si>
+    <t>Save this workbook as a Macro-Enabled Workbook (.xlsm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    File &gt; Save As &gt; Choose 'Excel Macro-Enabled Workbook (*.xlsm)'</t>
+  </si>
+  <si>
+    <t>Step 2:</t>
+  </si>
+  <si>
+    <t>Open the VBA Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Press Alt + F11 (Windows) or Option + F11 (Mac)</t>
+  </si>
+  <si>
+    <t>Step 3:</t>
+  </si>
+  <si>
+    <t>Insert a new Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Right-click on 'VBAProject' in the left panel &gt; Insert &gt; Module</t>
+  </si>
+  <si>
+    <t>Step 4:</t>
+  </si>
+  <si>
+    <t>Copy the VBA code below and paste it into the Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Select all the code in the 'COMPLETE VBA CODE' section below</t>
+  </si>
+  <si>
+    <t>Step 5:</t>
+  </si>
+  <si>
+    <t>Close the VBA Editor (File &gt; Close and Return to Microsoft Excel)</t>
+  </si>
+  <si>
+    <t>Step 6:</t>
+  </si>
+  <si>
+    <t>Create buttons on the Inputs sheet (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Developer tab &gt; Insert &gt; Button (Form Control) &gt; Draw button &gt; Assign macro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Create buttons for: LoadNRELLibrary, LoadLazardLibrary, LoadCPUCLibrary</t>
+  </si>
+  <si>
+    <t>Step 7:</t>
+  </si>
+  <si>
+    <t>Save the workbook again to preserve the macros</t>
+  </si>
+  <si>
+    <t>COMPLETE VBA CODE - COPY ALL BELOW</t>
+  </si>
+  <si>
+    <t>Option Explicit</t>
+  </si>
+  <si>
+    <t>'=================================================================</t>
+  </si>
+  <si>
+    <t>' BESS ANALYZER VBA MACROS</t>
+  </si>
+  <si>
+    <t>' Copy this entire module into your VBA project</t>
+  </si>
+  <si>
+    <t>Sub LoadNRELLibrary()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    '-----------------------------------------------------------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Loads NREL ATB 2024 Moderate assumptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    With ThisWorkbook.Sheets("Inputs")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Library name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C6").Value = "NREL ATB 2024 - Moderate"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Technology Specifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C18").Value = "LFP"          ' Chemistry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C19").Value = 0.85           ' Round-Trip Efficiency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C20").Value = 0.025          ' Annual Degradation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C21").Value = 6000           ' Cycle Life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C22").Value = 12             ' Augmentation Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C23").Value = 1              ' Cycles per Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Cost Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C28").Value = 160            ' CapEx ($/kWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C29").Value = 25             ' Fixed O&amp;M ($/kW-year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C30").Value = 0              ' Variable O&amp;M ($/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C31").Value = 55             ' Augmentation Cost ($/kWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C32").Value = 10             ' Decommissioning ($/kW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C33").Value = 30             ' Charging Cost ($/MWh)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C34").Value = 0.1            ' Residual Value (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Tax Credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C37").Value = 0.3            ' ITC Base (30%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C38").Value = 0              ' ITC Adders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Infrastructure Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C43").Value = 100            ' Interconnection ($/kW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C44").Value = 10             ' Land ($/kW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C45").Value = 15             ' Permitting ($/kW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C46").Value = 0.005          ' Insurance (% of CapEx)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C47").Value = 0.01           ' Property Tax (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Financing Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C51").Value = 0.6            ' Debt Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C52").Value = 0.045          ' Interest Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C53").Value = 15             ' Loan Term (years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C54").Value = 0.1            ' Cost of Equity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C55").Value = 0.21           ' Tax Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Benefits ($/kW-year and escalation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C59").Value = 150: .Range("D59").Value = 0.02   ' Resource Adequacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C60").Value = 40: .Range("D60").Value = 0.015   ' Energy Arbitrage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C61").Value = 15: .Range("D61").Value = 0.01    ' Ancillary Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C62").Value = 25: .Range("D62").Value = 0.02    ' T&amp;D Deferral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C63").Value = 50: .Range("D63").Value = 0.02    ' Resilience Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C64").Value = 25: .Range("D64").Value = 0.02    ' Renewable Integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C65").Value = 15: .Range("D65").Value = 0.03    ' GHG Emissions Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C66").Value = 8: .Range("D66").Value = 0.01     ' Voltage Support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    End With</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application.Calculate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "NREL ATB 2024 Moderate assumptions loaded successfully.", vbInformation, "Library Loaded"</t>
+  </si>
+  <si>
+    <t>End Sub</t>
+  </si>
+  <si>
+    <t>Sub LoadLazardLibrary()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Loads Lazard LCOS v10.0 2025 assumptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C6").Value = "Lazard LCOS 2025"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Technology</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C18").Value = "LFP"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C19").Value = 0.86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C20").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C21").Value = 6500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C22").Value = 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C23").Value = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Costs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C28").Value = 145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C29").Value = 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C30").Value = 0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C31").Value = 50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C32").Value = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C33").Value = 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C34").Value = 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C37").Value = 0.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C38").Value = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C43").Value = 90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C44").Value = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C45").Value = 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C46").Value = 0.005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C47").Value = 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Financing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C51").Value = 0.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C52").Value = 0.05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C53").Value = 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C54").Value = 0.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C55").Value = 0.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Benefits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C59").Value = 140: .Range("D59").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C60").Value = 45: .Range("D60").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C61").Value = 12: .Range("D61").Value = 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C62").Value = 20: .Range("D62").Value = 0.015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C63").Value = 45: .Range("D63").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C64").Value = 20: .Range("D64").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C65").Value = 12: .Range("D65").Value = 0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C66").Value = 6: .Range("D66").Value = 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "Lazard LCOS 2025 assumptions loaded successfully.", vbInformation, "Library Loaded"</t>
+  </si>
+  <si>
+    <t>Sub LoadCPUCLibrary()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Loads CPUC California 2024 assumptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Includes 10% ITC Energy Community Adder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C6").Value = "CPUC California 2024"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C19").Value = 0.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C20").Value = 0.025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C21").Value = 6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C28").Value = 155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C29").Value = 26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C30").Value = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C31").Value = 52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C32").Value = 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C33").Value = 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Tax Credits (includes Energy Community adder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C38").Value = 0.1            ' 10% Energy Community Adder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Infrastructure (California-specific higher costs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C43").Value = 120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C44").Value = 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C45").Value = 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C47").Value = 0.0105         ' CA property tax rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Financing (IOU-style favorable terms)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C51").Value = 0.65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C52").Value = 0.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C53").Value = 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C54").Value = 0.095</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        ' Benefits (California premium values)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C59").Value = 180: .Range("D59").Value = 0.025  ' RA premium in CA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C60").Value = 35: .Range("D60").Value = 0.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C61").Value = 10: .Range("D61").Value = 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C62").Value = 25: .Range("D62").Value = 0.015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C63").Value = 60: .Range("D63").Value = 0.02   ' PSPS resilience value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C64").Value = 30: .Range("D64").Value = 0.025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C65").Value = 20: .Range("D65").Value = 0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        .Range("C66").Value = 10: .Range("D66").Value = 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "CPUC California 2024 assumptions loaded." &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "Note: Includes 10% ITC Energy Community Adder.", vbInformation, "Library Loaded"</t>
+  </si>
+  <si>
+    <t>Sub GenerateReport()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Creates a summary report on a new "Report" sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim wsReport As Worksheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim wsResults As Worksheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim wsInputs As Worksheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim row As Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Set wsResults = ThisWorkbook.Sheets("Results")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Set wsInputs = ThisWorkbook.Sheets("Inputs")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Delete existing Report sheet if it exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    On Error Resume Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application.DisplayAlerts = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ThisWorkbook.Sheets("Report").Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application.DisplayAlerts = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    On Error GoTo 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Create new Report sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Set wsReport = ThisWorkbook.Sheets.Add(After:=ThisWorkbook.Sheets(ThisWorkbook.Sheets.Count))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Name = "Report"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    row = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "BESS ECONOMIC ANALYSIS REPORT"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Font.Bold = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Font.Size = 18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Range("B" &amp; row &amp; ":F" &amp; row).Merge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    row = row + 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Project Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "PROJECT SUMMARY"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Interior.Color = RGB(227, 242, 253)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    row = row + 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Project:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsInputs.Range("C7").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Location:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsInputs.Range("C9").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Capacity:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsInputs.Range("C10").Value &amp; " MW / " &amp; wsInputs.Range("C12").Value &amp; " MWh"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Assumptions:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsInputs.Range("C6").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Key Metrics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "KEY FINANCIAL METRICS"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Benefit-Cost Ratio (BCR):"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsResults.Range("C11").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).NumberFormat = "0.00"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Net Present Value (NPV):"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsResults.Range("C12").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).NumberFormat = "$#,##0"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Internal Rate of Return (IRR):"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsResults.Range("C13").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).NumberFormat = "0.0%"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "Payback Period:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsResults.Range("C14").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).NumberFormat = "0.0 "" years"""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "LCOS:"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).Value = wsResults.Range("C15").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 3).NumberFormat = "$#,##0 ""/MWh"""</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Recommendation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Cells(row, 2).Value = "RECOMMENDATION"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Color-code recommendation based on BCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim bcr As Double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    bcr = wsResults.Range("C11").Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    If bcr &gt;= 1.5 Then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Value = "STRONG PROJECT - Proceed with development"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Font.Color = RGB(0, 128, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ElseIf bcr &gt;= 1 Then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Value = "MARGINAL PROJECT - Review assumptions carefully"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Font.Color = RGB(255, 165, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Else</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Value = "NOT RECOMMENDED - Costs exceed benefits"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.Cells(row, 2).Font.Color = RGB(255, 0, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    End If</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Format columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Columns("B").ColumnWidth = 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wsReport.Columns("C").ColumnWidth = 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "Report generated on 'Report' sheet.", vbInformation, "Report Ready"</t>
+  </si>
+  <si>
+    <t>Sub ExportToPDF()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Exports the Report sheet to PDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Dim filePath As String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Set wsReport = ThisWorkbook.Sheets("Report")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    If wsReport Is Nothing Then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MsgBox "Please run 'Generate Report' first to create the Report sheet.", vbExclamation, "No Report Found"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Exit Sub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    filePath = Application.GetSaveAsFilename( _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        InitialFileName:="BESS_Analysis_Report.pdf", _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        FileFilter:="PDF Files (*.pdf), *.pdf", _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Title:="Save Report as PDF")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    If filePath &lt;&gt; "False" Then</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wsReport.ExportAsFixedFormat Type:=xlTypePDF, Filename:=filePath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        MsgBox "PDF exported successfully to:" &amp; vbCrLf &amp; filePath, vbInformation, "Export Complete"</t>
+  </si>
+  <si>
+    <t>Sub RefreshCalculations()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Forces recalculation of all formulas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Application.CalculateFull</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "All calculations refreshed.", vbInformation, "Refresh Complete"</t>
+  </si>
+  <si>
+    <t>Sub ShowAbout()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ' Shows information about the BESS Analyzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MsgBox "BESS Economic Analyzer" &amp; vbCrLf &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "Version: 1.0" &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "Libraries: NREL ATB 2024, Lazard LCOS 2025, CPUC CA 2024" &amp; vbCrLf &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "This tool performs benefit-cost analysis for utility-scale" &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "battery energy storage systems (BESS) using industry-standard" &amp; vbCrLf &amp; _</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           "assumptions and methodologies.", vbInformation, "About BESS Analyzer"</t>
+  </si>
+  <si>
+    <t>AVAILABLE MACROS - QUICK REFERENCE</t>
+  </si>
+  <si>
+    <t>LoadNRELLibrary</t>
+  </si>
+  <si>
+    <t>Loads NREL Annual Technology Baseline 2024 (Moderate) assumptions</t>
+  </si>
+  <si>
+    <t>LoadLazardLibrary</t>
+  </si>
+  <si>
+    <t>Loads Lazard Levelized Cost of Storage v10.0 (2025) assumptions</t>
+  </si>
+  <si>
+    <t>LoadCPUCLibrary</t>
+  </si>
+  <si>
+    <t>Loads CPUC California 2024 assumptions with 10% ITC Energy Community Adder</t>
+  </si>
+  <si>
+    <t>GenerateReport</t>
+  </si>
+  <si>
+    <t>Creates a summary report on a new 'Report' sheet</t>
+  </si>
+  <si>
+    <t>ExportToPDF</t>
+  </si>
+  <si>
+    <t>Exports the Report sheet to a PDF file</t>
+  </si>
+  <si>
+    <t>RefreshCalculations</t>
+  </si>
+  <si>
+    <t>Forces full recalculation of all workbook formulas</t>
+  </si>
+  <si>
+    <t>ShowAbout</t>
+  </si>
+  <si>
+    <t>Displays information about the BESS Analyzer</t>
+  </si>
+  <si>
+    <t>TROUBLESHOOTING</t>
+  </si>
+  <si>
+    <t>• If buttons don't work: Make sure you saved as .xlsm and macros are enabled</t>
+  </si>
+  <si>
+    <t>• If macros are disabled: Go to File &gt; Options &gt; Trust Center &gt; Trust Center Settings &gt; Macro Settings</t>
+  </si>
+  <si>
+    <t>• If cell references are wrong: The VBA code uses specific cell addresses - check the Inputs sheet layout</t>
+  </si>
+  <si>
+    <t>• To edit macros: Press Alt+F11 to open VBA Editor, then modify the code in the Module</t>
+  </si>
+  <si>
+    <t>• To assign macros to buttons: Right-click button &gt; Assign Macro &gt; Select from list</t>
   </si>
 </sst>
 </file>
@@ -975,7 +1792,7 @@
     <numFmt numFmtId="168" formatCode="0.0"/>
     <numFmt numFmtId="169" formatCode="$#,##0,,&quot;M&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1031,8 +1848,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1063,8 +1886,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1087,11 +1916,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1126,6 +1970,10 @@
     <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6126,4 +6974,1809 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:C374"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="20" t="s">
+        <v>316</v>
+      </c>
+      <c r="C6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="20" t="s">
+        <v>319</v>
+      </c>
+      <c r="C8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="5" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="20" t="s">
+        <v>325</v>
+      </c>
+      <c r="C12" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="20" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="5" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="C16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="21" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="21" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="21" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="B27" s="21"/>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="B28" s="21" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3">
+      <c r="B30" s="21" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="B32" s="21" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" s="21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="21"/>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="21" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" s="21" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" s="21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" s="21" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" s="21" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2">
+      <c r="B42" s="21" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="21"/>
+    </row>
+    <row r="44" spans="2:2">
+      <c r="B44" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2">
+      <c r="B45" s="21" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
+      <c r="B46" s="21" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="21" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="21" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" s="21" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2">
+      <c r="B51" s="21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2">
+      <c r="B52" s="21"/>
+    </row>
+    <row r="53" spans="2:2">
+      <c r="B53" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2">
+      <c r="B54" s="21" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2">
+      <c r="B55" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2">
+      <c r="B56" s="21"/>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="21" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="21" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="21" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="21" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="21"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="21" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="21" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="21" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="21" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" s="21" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2">
+      <c r="B70" s="21"/>
+    </row>
+    <row r="71" spans="2:2">
+      <c r="B71" s="21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2">
+      <c r="B72" s="21" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2">
+      <c r="B73" s="21" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2">
+      <c r="B74" s="21" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2">
+      <c r="B75" s="21" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2">
+      <c r="B76" s="21" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2">
+      <c r="B77" s="21" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2">
+      <c r="B78" s="21" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2">
+      <c r="B79" s="21" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2">
+      <c r="B80" s="21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2">
+      <c r="B81" s="21"/>
+    </row>
+    <row r="82" spans="2:2">
+      <c r="B82" s="21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2">
+      <c r="B83" s="21" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2">
+      <c r="B84" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2">
+      <c r="B85" s="21"/>
+    </row>
+    <row r="86" spans="2:2">
+      <c r="B86" s="21"/>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" s="21" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2">
+      <c r="B88" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2">
+      <c r="B89" s="21" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2">
+      <c r="B90" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2">
+      <c r="B91" s="21" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2">
+      <c r="B92" s="21" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" s="21"/>
+    </row>
+    <row r="94" spans="2:2">
+      <c r="B94" s="21" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2">
+      <c r="B95" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2">
+      <c r="B96" s="21" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2">
+      <c r="B97" s="21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2">
+      <c r="B98" s="21" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" s="21" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2">
+      <c r="B100" s="21" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2">
+      <c r="B101" s="21"/>
+    </row>
+    <row r="102" spans="2:2">
+      <c r="B102" s="21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2">
+      <c r="B103" s="21" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" s="21" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" s="21" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2">
+      <c r="B106" s="21" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2">
+      <c r="B107" s="21" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2">
+      <c r="B108" s="21" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2">
+      <c r="B109" s="21" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2">
+      <c r="B110" s="21"/>
+    </row>
+    <row r="111" spans="2:2">
+      <c r="B111" s="21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2">
+      <c r="B112" s="21" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2">
+      <c r="B113" s="21" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2">
+      <c r="B114" s="21"/>
+    </row>
+    <row r="115" spans="2:2">
+      <c r="B115" s="21" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" s="21" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" s="21" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" s="21" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" s="21" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="21" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" s="21"/>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" s="21" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" s="21" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" s="21" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" s="21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" s="21" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" s="21" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" s="21"/>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" s="21" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" s="21" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" s="21" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" s="21" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="21" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" s="21" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" s="21" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" s="21" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" s="21" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" s="21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" s="21"/>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" s="21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" s="21" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" s="21"/>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" s="21"/>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145" s="21" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2">
+      <c r="B146" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2">
+      <c r="B147" s="21" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2">
+      <c r="B148" s="21" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2">
+      <c r="B149" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2">
+      <c r="B150" s="21" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2">
+      <c r="B151" s="21" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2">
+      <c r="B152" s="21"/>
+    </row>
+    <row r="153" spans="2:2">
+      <c r="B153" s="21" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2">
+      <c r="B154" s="21" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2">
+      <c r="B155" s="21" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2">
+      <c r="B156" s="21" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2">
+      <c r="B157" s="21" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2">
+      <c r="B158" s="21" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2">
+      <c r="B159" s="21" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2">
+      <c r="B160" s="21"/>
+    </row>
+    <row r="161" spans="2:2">
+      <c r="B161" s="21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" s="21" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163" s="21" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" s="21" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165" s="21" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" s="21" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" s="21" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2">
+      <c r="B168" s="21" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2">
+      <c r="B169" s="21"/>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" s="21" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" s="21" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" s="21" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" s="21"/>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" s="21" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" s="21" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" s="21" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2">
+      <c r="B177" s="21" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" s="21" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2">
+      <c r="B179" s="21" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2">
+      <c r="B180" s="21"/>
+    </row>
+    <row r="181" spans="2:2">
+      <c r="B181" s="21" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2">
+      <c r="B182" s="21" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2">
+      <c r="B183" s="21" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2">
+      <c r="B184" s="21" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" s="21" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" s="21" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" s="21"/>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" s="21" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" s="21" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" s="21" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2">
+      <c r="B191" s="21" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" s="21" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2">
+      <c r="B193" s="21" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2">
+      <c r="B194" s="21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2">
+      <c r="B195" s="21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="196" spans="2:2">
+      <c r="B196" s="21" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="197" spans="2:2">
+      <c r="B197" s="21" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2">
+      <c r="B198" s="21"/>
+    </row>
+    <row r="199" spans="2:2">
+      <c r="B199" s="21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2">
+      <c r="B200" s="21" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2">
+      <c r="B201" s="21" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2">
+      <c r="B202" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2">
+      <c r="B203" s="21"/>
+    </row>
+    <row r="204" spans="2:2">
+      <c r="B204" s="21"/>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" s="21" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="206" spans="2:2">
+      <c r="B206" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="207" spans="2:2">
+      <c r="B207" s="21" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="208" spans="2:2">
+      <c r="B208" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209" s="21" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="210" spans="2:2">
+      <c r="B210" s="21" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="211" spans="2:2">
+      <c r="B211" s="21" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2">
+      <c r="B212" s="21" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2">
+      <c r="B213" s="21"/>
+    </row>
+    <row r="214" spans="2:2">
+      <c r="B214" s="21" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2">
+      <c r="B215" s="21" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2">
+      <c r="B216" s="21"/>
+    </row>
+    <row r="217" spans="2:2">
+      <c r="B217" s="21" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="218" spans="2:2">
+      <c r="B218" s="21" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="219" spans="2:2">
+      <c r="B219" s="21" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2">
+      <c r="B220" s="21" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2">
+      <c r="B221" s="21" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2">
+      <c r="B222" s="21" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2">
+      <c r="B223" s="21"/>
+    </row>
+    <row r="224" spans="2:2">
+      <c r="B224" s="21" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2">
+      <c r="B225" s="21" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2">
+      <c r="B226" s="21" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2">
+      <c r="B227" s="21"/>
+    </row>
+    <row r="228" spans="2:2">
+      <c r="B228" s="21" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2">
+      <c r="B229" s="21" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2">
+      <c r="B230" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2">
+      <c r="B231" s="21" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2">
+      <c r="B232" s="21" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2">
+      <c r="B233" s="21" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2">
+      <c r="B234" s="21"/>
+    </row>
+    <row r="235" spans="2:2">
+      <c r="B235" s="21" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2">
+      <c r="B236" s="21" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2">
+      <c r="B237" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2">
+      <c r="B238" s="21" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2">
+      <c r="B240" s="21"/>
+    </row>
+    <row r="241" spans="2:2">
+      <c r="B241" s="21" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="242" spans="2:2">
+      <c r="B242" s="21" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="243" spans="2:2">
+      <c r="B243" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2">
+      <c r="B244" s="21" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="245" spans="2:2">
+      <c r="B245" s="21" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="246" spans="2:2">
+      <c r="B246" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="247" spans="2:2">
+      <c r="B247" s="21" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="248" spans="2:2">
+      <c r="B248" s="21" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="249" spans="2:2">
+      <c r="B249" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="250" spans="2:2">
+      <c r="B250" s="21" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="251" spans="2:2">
+      <c r="B251" s="21" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="252" spans="2:2">
+      <c r="B252" s="21" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="253" spans="2:2">
+      <c r="B253" s="21"/>
+    </row>
+    <row r="254" spans="2:2">
+      <c r="B254" s="21" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="255" spans="2:2">
+      <c r="B255" s="21" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="256" spans="2:2">
+      <c r="B256" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="257" spans="2:2">
+      <c r="B257" s="21" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="258" spans="2:2">
+      <c r="B258" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="259" spans="2:2">
+      <c r="B259" s="21"/>
+    </row>
+    <row r="260" spans="2:2">
+      <c r="B260" s="21" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="261" spans="2:2">
+      <c r="B261" s="21" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="262" spans="2:2">
+      <c r="B262" s="21" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2">
+      <c r="B263" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="264" spans="2:2">
+      <c r="B264" s="21" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="265" spans="2:2">
+      <c r="B265" s="21" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="266" spans="2:2">
+      <c r="B266" s="21" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="267" spans="2:2">
+      <c r="B267" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="268" spans="2:2">
+      <c r="B268" s="21" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="269" spans="2:2">
+      <c r="B269" s="21" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="270" spans="2:2">
+      <c r="B270" s="21" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="271" spans="2:2">
+      <c r="B271" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="272" spans="2:2">
+      <c r="B272" s="21" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" s="21" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2">
+      <c r="B274" s="21" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2">
+      <c r="B275" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2">
+      <c r="B276" s="21" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2">
+      <c r="B277" s="21" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2">
+      <c r="B278" s="21" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2">
+      <c r="B279" s="21" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2">
+      <c r="B280" s="21"/>
+    </row>
+    <row r="281" spans="2:2">
+      <c r="B281" s="21" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2">
+      <c r="B282" s="21" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2">
+      <c r="B283" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2">
+      <c r="B284" s="21" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2">
+      <c r="B285" s="21" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2">
+      <c r="B286" s="21"/>
+    </row>
+    <row r="287" spans="2:2">
+      <c r="B287" s="21" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2">
+      <c r="B288" s="21" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2">
+      <c r="B289" s="21" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2">
+      <c r="B290" s="21" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2">
+      <c r="B291" s="21" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2">
+      <c r="B292" s="21" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2">
+      <c r="B293" s="21" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2">
+      <c r="B294" s="21" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2">
+      <c r="B295" s="21" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2">
+      <c r="B296" s="21" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2">
+      <c r="B297" s="21" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2">
+      <c r="B298" s="21" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2">
+      <c r="B299" s="21" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2">
+      <c r="B300" s="21" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="301" spans="2:2">
+      <c r="B301" s="21"/>
+    </row>
+    <row r="302" spans="2:2">
+      <c r="B302" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="303" spans="2:2">
+      <c r="B303" s="21" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="304" spans="2:2">
+      <c r="B304" s="21" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="305" spans="2:2">
+      <c r="B305" s="21"/>
+    </row>
+    <row r="306" spans="2:2">
+      <c r="B306" s="21" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="307" spans="2:2">
+      <c r="B307" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="308" spans="2:2">
+      <c r="B308" s="21"/>
+    </row>
+    <row r="309" spans="2:2">
+      <c r="B309" s="21"/>
+    </row>
+    <row r="310" spans="2:2">
+      <c r="B310" s="21" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="311" spans="2:2">
+      <c r="B311" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="312" spans="2:2">
+      <c r="B312" s="21" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="313" spans="2:2">
+      <c r="B313" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="314" spans="2:2">
+      <c r="B314" s="21" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="315" spans="2:2">
+      <c r="B315" s="21" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="316" spans="2:2">
+      <c r="B316" s="21"/>
+    </row>
+    <row r="317" spans="2:2">
+      <c r="B317" s="21" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="318" spans="2:2">
+      <c r="B318" s="21" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="319" spans="2:2">
+      <c r="B319" s="21" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="320" spans="2:2">
+      <c r="B320" s="21"/>
+    </row>
+    <row r="321" spans="2:2">
+      <c r="B321" s="21" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="322" spans="2:2">
+      <c r="B322" s="21" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="323" spans="2:2">
+      <c r="B323" s="21" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="324" spans="2:2">
+      <c r="B324" s="21" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="325" spans="2:2">
+      <c r="B325" s="21"/>
+    </row>
+    <row r="326" spans="2:2">
+      <c r="B326" s="21" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="327" spans="2:2">
+      <c r="B327" s="21" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="328" spans="2:2">
+      <c r="B328" s="21" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="329" spans="2:2">
+      <c r="B329" s="21" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="330" spans="2:2">
+      <c r="B330" s="21"/>
+    </row>
+    <row r="331" spans="2:2">
+      <c r="B331" s="21" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="332" spans="2:2">
+      <c r="B332" s="21" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="333" spans="2:2">
+      <c r="B333" s="21" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="334" spans="2:2">
+      <c r="B334" s="21" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="335" spans="2:2">
+      <c r="B335" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="336" spans="2:2">
+      <c r="B336" s="21"/>
+    </row>
+    <row r="337" spans="2:2">
+      <c r="B337" s="21"/>
+    </row>
+    <row r="338" spans="2:2">
+      <c r="B338" s="21" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="339" spans="2:2">
+      <c r="B339" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="340" spans="2:2">
+      <c r="B340" s="21" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="341" spans="2:2">
+      <c r="B341" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="342" spans="2:2">
+      <c r="B342" s="21" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="343" spans="2:2">
+      <c r="B343" s="21" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="344" spans="2:2">
+      <c r="B344" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="345" spans="2:2">
+      <c r="B345" s="21"/>
+    </row>
+    <row r="346" spans="2:2">
+      <c r="B346" s="21"/>
+    </row>
+    <row r="347" spans="2:2">
+      <c r="B347" s="21" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="348" spans="2:2">
+      <c r="B348" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="349" spans="2:2">
+      <c r="B349" s="21" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="350" spans="2:2">
+      <c r="B350" s="21" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="351" spans="2:2">
+      <c r="B351" s="21" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="352" spans="2:2">
+      <c r="B352" s="21" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="353" spans="2:3">
+      <c r="B353" s="21" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="354" spans="2:3">
+      <c r="B354" s="21" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="355" spans="2:3">
+      <c r="B355" s="21" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="356" spans="2:3">
+      <c r="B356" s="21" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="357" spans="2:3">
+      <c r="B357" s="21" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="359" spans="2:3">
+      <c r="B359" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="C359" s="2"/>
+    </row>
+    <row r="360" spans="2:3">
+      <c r="B360" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C360" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="361" spans="2:3">
+      <c r="B361" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C361" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="362" spans="2:3">
+      <c r="B362" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="C362" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="363" spans="2:3">
+      <c r="B363" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="C363" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="364" spans="2:3">
+      <c r="B364" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="C364" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="365" spans="2:3">
+      <c r="B365" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="C365" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="366" spans="2:3">
+      <c r="B366" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="C366" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="369" spans="2:3">
+      <c r="B369" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C369" s="2"/>
+    </row>
+    <row r="370" spans="2:3">
+      <c r="B370" s="5" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="371" spans="2:3">
+      <c r="B371" s="5" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="372" spans="2:3">
+      <c r="B372" s="5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="373" spans="2:3">
+      <c r="B373" s="5" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="374" spans="2:3">
+      <c r="B374" s="5" t="s">
+        <v>582</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B359:C359"/>
+    <mergeCell ref="B369:C369"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>